<commit_message>
primeiro codigo do robo da bahia
</commit_message>
<xml_diff>
--- a/BASE_DADOS.xlsx
+++ b/BASE_DADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1077"/>
+  <dimension ref="A1:G1110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31226,6 +31226,963 @@
         </is>
       </c>
     </row>
+    <row r="1078">
+      <c r="A1078" t="n">
+        <v>2050419</v>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 09/01/24</t>
+        </is>
+      </c>
+      <c r="C1078" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1078" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1078" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1078" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1078" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="n">
+        <v>2050435</v>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 09/01/24</t>
+        </is>
+      </c>
+      <c r="C1079" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1079" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1079" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1079" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1079" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="n">
+        <v>2050447</v>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 09/01/24</t>
+        </is>
+      </c>
+      <c r="C1080" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1080" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1080" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1080" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1080" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="n">
+        <v>2050460</v>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 09/01/24</t>
+        </is>
+      </c>
+      <c r="C1081" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1081" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1081" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1081" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1081" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="n">
+        <v>2050464</v>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 09/01/24</t>
+        </is>
+      </c>
+      <c r="C1082" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1082" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1082" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1082" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1082" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="n">
+        <v>2057337</v>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1083" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1083" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1083" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1083" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1083" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="n">
+        <v>2057380</v>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1084" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1084" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1084" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1084" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1084" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="n">
+        <v>2057393</v>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1085" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1085" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1085" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1085" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1085" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="n">
+        <v>2057441</v>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1086" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1086" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1086" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1086" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1086" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="n">
+        <v>2057463</v>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1087" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1087" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1087" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1087" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1087" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="n">
+        <v>2057474</v>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1088" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1088" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1088" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1088" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1088" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="n">
+        <v>1243111</v>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1089" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1089" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1089" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1089" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1089" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="n">
+        <v>2055535</v>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1090" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1090" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1090" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1090" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1090" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="n">
+        <v>2055536</v>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1091" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1091" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1091" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1091" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1091" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="n">
+        <v>2055555</v>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1092" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1092" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1092" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1092" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1092" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="n">
+        <v>2055556</v>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1093" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1093" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1093" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1093" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1093" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="n">
+        <v>2055561</v>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1094" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1094" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1094" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1094" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1094" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="n">
+        <v>2055562</v>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1095" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1095" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1095" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1095" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1095" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="n">
+        <v>2057261</v>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1096" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1096" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1096" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1096" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1096" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="n">
+        <v>2057328</v>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1097" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1097" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1097" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1097" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1097" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="n">
+        <v>2057372</v>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1098" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1098" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1098" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1098" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1098" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="n">
+        <v>2057381</v>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1099" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1099" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1099" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1099" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1099" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="n">
+        <v>2057382</v>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1100" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1100" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1100" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1100" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1100" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="n">
+        <v>2057383</v>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1101" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1101" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1101" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1101" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1101" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="n">
+        <v>2059012</v>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17/01/24</t>
+        </is>
+      </c>
+      <c r="C1102" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1102" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1102" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1102" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1102" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="n">
+        <v>2055492</v>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1103" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1103" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1103" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1103" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1103" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="n">
+        <v>2055493</v>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1104" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1104" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1104" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1104" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1104" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="n">
+        <v>2057284</v>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/01/24</t>
+        </is>
+      </c>
+      <c r="C1105" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1105" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1105" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1105" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1105" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="n">
+        <v>2055511</v>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1106" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1106" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1106" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1106" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1106" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="n">
+        <v>2055532</v>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1107" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1107" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1107" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1107" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1107" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="n">
+        <v>2055559</v>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1108" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1108" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1108" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1108" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1108" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="n">
+        <v>2055560</v>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1109" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1109" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1109" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1109" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1109" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="n">
+        <v>2055567</v>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/01/24</t>
+        </is>
+      </c>
+      <c r="C1110" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="D1110" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="E1110" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="F1110" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G1110" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
atualizado com o onedrive
</commit_message>
<xml_diff>
--- a/BASE_DADOS.xlsx
+++ b/BASE_DADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2146"/>
+  <dimension ref="A1:G2240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68437,6 +68437,3296 @@
         </is>
       </c>
     </row>
+    <row r="2147">
+      <c r="A2147" t="n">
+        <v>1469483</v>
+      </c>
+      <c r="B2147" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2147" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2147" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2147" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2147" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2147" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2148">
+      <c r="A2148" t="n">
+        <v>1469484</v>
+      </c>
+      <c r="B2148" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2148" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2148" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2148" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2148" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2148" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2149">
+      <c r="A2149" t="n">
+        <v>1469485</v>
+      </c>
+      <c r="B2149" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2149" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2149" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2149" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2149" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2149" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2150">
+      <c r="A2150" t="n">
+        <v>1469486</v>
+      </c>
+      <c r="B2150" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2150" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2150" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2150" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2150" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2150" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2151">
+      <c r="A2151" t="n">
+        <v>1469487</v>
+      </c>
+      <c r="B2151" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2151" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2151" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2151" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2151" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2151" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2152">
+      <c r="A2152" t="n">
+        <v>1469488</v>
+      </c>
+      <c r="B2152" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2152" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2152" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2152" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2152" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2152" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2153">
+      <c r="A2153" t="n">
+        <v>1469497</v>
+      </c>
+      <c r="B2153" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2153" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2153" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2153" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2153" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2153" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2154">
+      <c r="A2154" t="n">
+        <v>1469498</v>
+      </c>
+      <c r="B2154" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2154" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2154" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2154" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2154" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2154" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2155">
+      <c r="A2155" t="n">
+        <v>1469499</v>
+      </c>
+      <c r="B2155" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2155" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2155" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2155" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2155" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2155" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2156">
+      <c r="A2156" t="n">
+        <v>1460444</v>
+      </c>
+      <c r="B2156" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2156" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2156" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2156" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2156" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2156" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2157">
+      <c r="A2157" t="n">
+        <v>1460445</v>
+      </c>
+      <c r="B2157" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2157" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2157" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2157" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2157" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2157" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2158">
+      <c r="A2158" t="n">
+        <v>1460446</v>
+      </c>
+      <c r="B2158" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2158" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2158" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2158" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2158" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2158" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2159">
+      <c r="A2159" t="n">
+        <v>1460585</v>
+      </c>
+      <c r="B2159" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2159" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2159" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2159" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2159" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2159" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2160">
+      <c r="A2160" t="n">
+        <v>1460586</v>
+      </c>
+      <c r="B2160" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2160" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2160" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2160" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2160" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2160" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2161">
+      <c r="A2161" t="n">
+        <v>1460587</v>
+      </c>
+      <c r="B2161" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2161" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2161" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2161" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2161" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2161" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2162">
+      <c r="A2162" t="n">
+        <v>1460588</v>
+      </c>
+      <c r="B2162" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2162" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2162" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2162" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2162" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2162" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2163">
+      <c r="A2163" t="n">
+        <v>1460759</v>
+      </c>
+      <c r="B2163" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2163" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2163" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2163" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2163" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2163" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2164">
+      <c r="A2164" t="n">
+        <v>1460760</v>
+      </c>
+      <c r="B2164" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2164" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2164" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2164" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2164" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2164" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2165">
+      <c r="A2165" t="n">
+        <v>1460761</v>
+      </c>
+      <c r="B2165" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2165" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2165" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2165" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2165" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2165" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2166">
+      <c r="A2166" t="n">
+        <v>1460762</v>
+      </c>
+      <c r="B2166" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2166" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2166" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2166" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2166" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2166" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2167">
+      <c r="A2167" t="n">
+        <v>1460763</v>
+      </c>
+      <c r="B2167" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2167" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2167" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2167" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2167" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2167" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2168">
+      <c r="A2168" t="n">
+        <v>1460764</v>
+      </c>
+      <c r="B2168" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2168" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2168" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2168" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2168" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2168" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2169">
+      <c r="A2169" t="n">
+        <v>1460788</v>
+      </c>
+      <c r="B2169" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2169" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2169" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2169" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2169" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2169" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2170">
+      <c r="A2170" t="n">
+        <v>1460789</v>
+      </c>
+      <c r="B2170" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2170" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2170" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2170" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2170" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2170" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2171">
+      <c r="A2171" t="n">
+        <v>1460790</v>
+      </c>
+      <c r="B2171" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2171" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2171" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2171" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2171" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2171" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2172">
+      <c r="A2172" t="n">
+        <v>1460879</v>
+      </c>
+      <c r="B2172" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2172" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2172" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2172" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2172" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2172" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2173">
+      <c r="A2173" t="n">
+        <v>1460880</v>
+      </c>
+      <c r="B2173" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2173" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2173" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2173" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2173" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2173" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2174">
+      <c r="A2174" t="n">
+        <v>1460881</v>
+      </c>
+      <c r="B2174" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2174" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2174" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2174" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2174" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2174" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2175">
+      <c r="A2175" t="n">
+        <v>1460946</v>
+      </c>
+      <c r="B2175" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2175" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2175" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2175" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2175" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2175" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2176">
+      <c r="A2176" t="n">
+        <v>1460948</v>
+      </c>
+      <c r="B2176" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2176" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2176" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2176" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2176" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2176" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2177">
+      <c r="A2177" t="n">
+        <v>1461042</v>
+      </c>
+      <c r="B2177" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2177" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2177" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2177" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2177" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2177" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" t="n">
+        <v>1461043</v>
+      </c>
+      <c r="B2178" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2178" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2178" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2178" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2178" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2178" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" t="n">
+        <v>1461044</v>
+      </c>
+      <c r="B2179" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2179" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2179" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2179" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2179" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2179" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" t="n">
+        <v>1461045</v>
+      </c>
+      <c r="B2180" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2180" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2180" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2180" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2180" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2180" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" t="n">
+        <v>1461046</v>
+      </c>
+      <c r="B2181" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2181" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2181" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2181" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2181" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2181" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" t="n">
+        <v>1461047</v>
+      </c>
+      <c r="B2182" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2182" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2182" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2182" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2182" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2182" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" t="n">
+        <v>1461048</v>
+      </c>
+      <c r="B2183" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2183" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2183" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2183" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2183" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2183" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" t="n">
+        <v>1461060</v>
+      </c>
+      <c r="B2184" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2184" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2184" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2184" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2184" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2184" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" t="n">
+        <v>1461115</v>
+      </c>
+      <c r="B2185" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2185" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2185" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2185" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2185" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2185" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" t="n">
+        <v>1461116</v>
+      </c>
+      <c r="B2186" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2186" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2186" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2186" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2186" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2186" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" t="n">
+        <v>1461117</v>
+      </c>
+      <c r="B2187" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2187" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2187" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2187" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2187" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2187" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" t="n">
+        <v>1469009</v>
+      </c>
+      <c r="B2188" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2188" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2188" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2188" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2188" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2188" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2189">
+      <c r="A2189" t="n">
+        <v>1469010</v>
+      </c>
+      <c r="B2189" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2189" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2189" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2189" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2189" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2189" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2190">
+      <c r="A2190" t="n">
+        <v>1469011</v>
+      </c>
+      <c r="B2190" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2190" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2190" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2190" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2190" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2190" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2191">
+      <c r="A2191" t="n">
+        <v>1469012</v>
+      </c>
+      <c r="B2191" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2191" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2191" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2191" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2191" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2191" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2192">
+      <c r="A2192" t="n">
+        <v>1469013</v>
+      </c>
+      <c r="B2192" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2192" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2192" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2192" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2192" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2192" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2193">
+      <c r="A2193" t="n">
+        <v>1469024</v>
+      </c>
+      <c r="B2193" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2193" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2193" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2193" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2193" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2193" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2194">
+      <c r="A2194" t="n">
+        <v>1469028</v>
+      </c>
+      <c r="B2194" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2194" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2194" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2194" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2194" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2194" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2195">
+      <c r="A2195" t="n">
+        <v>1469029</v>
+      </c>
+      <c r="B2195" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2195" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2195" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2195" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2195" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2195" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2196">
+      <c r="A2196" t="n">
+        <v>1469087</v>
+      </c>
+      <c r="B2196" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2196" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2196" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2196" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2196" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2196" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2197">
+      <c r="A2197" t="n">
+        <v>1469088</v>
+      </c>
+      <c r="B2197" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2197" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2197" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2197" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2197" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2197" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2198">
+      <c r="A2198" t="n">
+        <v>1469089</v>
+      </c>
+      <c r="B2198" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2198" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2198" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2198" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2198" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2198" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2199">
+      <c r="A2199" t="n">
+        <v>1469090</v>
+      </c>
+      <c r="B2199" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2199" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2199" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2199" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2199" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2199" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2200">
+      <c r="A2200" t="n">
+        <v>1469097</v>
+      </c>
+      <c r="B2200" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2200" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2200" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2200" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2200" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2200" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2201">
+      <c r="A2201" t="n">
+        <v>1469098</v>
+      </c>
+      <c r="B2201" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2201" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2201" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2201" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2201" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2201" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2202">
+      <c r="A2202" t="n">
+        <v>1469104</v>
+      </c>
+      <c r="B2202" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2202" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2202" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2202" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2202" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2202" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2203">
+      <c r="A2203" t="n">
+        <v>1469105</v>
+      </c>
+      <c r="B2203" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2203" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2203" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2203" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2203" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2203" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2204">
+      <c r="A2204" t="n">
+        <v>1469106</v>
+      </c>
+      <c r="B2204" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2204" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2204" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2204" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2204" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2204" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2205">
+      <c r="A2205" t="n">
+        <v>1469144</v>
+      </c>
+      <c r="B2205" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2205" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2205" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2205" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2205" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2205" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2206">
+      <c r="A2206" t="n">
+        <v>1469146</v>
+      </c>
+      <c r="B2206" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2206" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2206" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2206" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2206" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2206" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2207">
+      <c r="A2207" t="n">
+        <v>1469153</v>
+      </c>
+      <c r="B2207" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2207" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2207" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2207" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2207" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2207" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2208">
+      <c r="A2208" t="n">
+        <v>1469154</v>
+      </c>
+      <c r="B2208" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2208" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2208" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2208" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2208" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2208" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2209">
+      <c r="A2209" t="n">
+        <v>1469155</v>
+      </c>
+      <c r="B2209" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2209" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2209" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2209" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2209" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2209" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2210">
+      <c r="A2210" t="n">
+        <v>1469222</v>
+      </c>
+      <c r="B2210" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2210" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2210" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2210" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2210" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2210" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2211">
+      <c r="A2211" t="n">
+        <v>1469223</v>
+      </c>
+      <c r="B2211" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2211" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2211" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2211" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2211" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2211" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2212">
+      <c r="A2212" t="n">
+        <v>1469224</v>
+      </c>
+      <c r="B2212" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2212" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2212" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2212" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2212" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2212" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2213">
+      <c r="A2213" t="n">
+        <v>1469225</v>
+      </c>
+      <c r="B2213" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2213" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2213" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2213" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2213" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2213" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2214">
+      <c r="A2214" t="n">
+        <v>1469226</v>
+      </c>
+      <c r="B2214" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2214" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2214" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2214" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2214" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2214" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2215">
+      <c r="A2215" t="n">
+        <v>1469227</v>
+      </c>
+      <c r="B2215" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2215" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2215" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2215" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2215" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2215" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2216">
+      <c r="A2216" t="n">
+        <v>1469228</v>
+      </c>
+      <c r="B2216" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2216" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2216" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2216" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2216" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2216" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2217">
+      <c r="A2217" t="n">
+        <v>1469241</v>
+      </c>
+      <c r="B2217" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2217" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2217" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2217" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2217" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2217" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2218">
+      <c r="A2218" t="n">
+        <v>1469300</v>
+      </c>
+      <c r="B2218" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2218" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2218" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2218" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2218" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2218" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2219">
+      <c r="A2219" t="n">
+        <v>1469301</v>
+      </c>
+      <c r="B2219" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2219" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2219" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2219" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2219" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2219" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2220">
+      <c r="A2220" t="n">
+        <v>1469302</v>
+      </c>
+      <c r="B2220" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2220" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2220" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2220" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2220" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2220" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2221">
+      <c r="A2221" t="n">
+        <v>1469343</v>
+      </c>
+      <c r="B2221" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2221" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2221" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2221" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2221" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2221" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2222">
+      <c r="A2222" t="n">
+        <v>1469344</v>
+      </c>
+      <c r="B2222" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2222" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2222" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2222" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2222" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2222" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2223">
+      <c r="A2223" t="n">
+        <v>1469345</v>
+      </c>
+      <c r="B2223" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2223" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2223" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2223" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2223" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2223" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2224">
+      <c r="A2224" t="n">
+        <v>1469462</v>
+      </c>
+      <c r="B2224" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2224" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2224" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2224" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2224" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2224" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2225">
+      <c r="A2225" t="n">
+        <v>1469463</v>
+      </c>
+      <c r="B2225" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2225" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2225" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2225" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2225" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2225" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2226">
+      <c r="A2226" t="n">
+        <v>1469464</v>
+      </c>
+      <c r="B2226" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2226" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2226" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2226" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2226" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2226" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2227">
+      <c r="A2227" t="n">
+        <v>1450321</v>
+      </c>
+      <c r="B2227" t="inlineStr">
+        <is>
+          <t>21/05/2024</t>
+        </is>
+      </c>
+      <c r="C2227" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2227" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2227" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2227" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2227" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2228">
+      <c r="A2228" t="n">
+        <v>1450322</v>
+      </c>
+      <c r="B2228" t="inlineStr">
+        <is>
+          <t>21/05/2024</t>
+        </is>
+      </c>
+      <c r="C2228" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2228" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2228" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2228" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2228" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2229">
+      <c r="A2229" t="n">
+        <v>1450323</v>
+      </c>
+      <c r="B2229" t="inlineStr">
+        <is>
+          <t>21/05/2024</t>
+        </is>
+      </c>
+      <c r="C2229" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2229" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2229" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2229" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2229" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2230">
+      <c r="A2230" t="n">
+        <v>1450324</v>
+      </c>
+      <c r="B2230" t="inlineStr">
+        <is>
+          <t>21/05/2024</t>
+        </is>
+      </c>
+      <c r="C2230" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2230" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2230" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2230" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2230" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2231">
+      <c r="A2231" t="n">
+        <v>1453645</v>
+      </c>
+      <c r="B2231" t="inlineStr">
+        <is>
+          <t>22/05/2024</t>
+        </is>
+      </c>
+      <c r="C2231" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2231" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2231" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2231" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2231" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2232">
+      <c r="A2232" t="n">
+        <v>1453646</v>
+      </c>
+      <c r="B2232" t="inlineStr">
+        <is>
+          <t>22/05/2024</t>
+        </is>
+      </c>
+      <c r="C2232" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2232" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2232" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2232" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2232" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2233">
+      <c r="A2233" t="n">
+        <v>1460091</v>
+      </c>
+      <c r="B2233" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2233" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2233" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2233" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2233" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2233" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2234">
+      <c r="A2234" t="n">
+        <v>1460418</v>
+      </c>
+      <c r="B2234" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2234" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2234" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2234" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2234" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2234" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2235">
+      <c r="A2235" t="n">
+        <v>1460419</v>
+      </c>
+      <c r="B2235" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2235" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2235" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2235" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2235" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2235" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2236">
+      <c r="A2236" t="n">
+        <v>1460420</v>
+      </c>
+      <c r="B2236" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2236" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2236" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2236" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2236" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2236" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2237">
+      <c r="A2237" t="n">
+        <v>1460538</v>
+      </c>
+      <c r="B2237" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2237" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2237" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2237" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2237" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2237" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2238">
+      <c r="A2238" t="n">
+        <v>1460539</v>
+      </c>
+      <c r="B2238" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2238" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2238" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2238" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2238" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2238" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2239">
+      <c r="A2239" t="n">
+        <v>1460540</v>
+      </c>
+      <c r="B2239" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2239" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2239" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2239" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2239" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2239" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2240">
+      <c r="A2240" t="n">
+        <v>1460600</v>
+      </c>
+      <c r="B2240" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2240" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2240" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2240" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2240" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2240" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
atualizado com verificação de ok no final
</commit_message>
<xml_diff>
--- a/BASE_DADOS.xlsx
+++ b/BASE_DADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2240"/>
+  <dimension ref="A1:G2317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -71727,6 +71727,2701 @@
         </is>
       </c>
     </row>
+    <row r="2241">
+      <c r="A2241" t="n">
+        <v>1460601</v>
+      </c>
+      <c r="B2241" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2241" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2241" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2241" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2241" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2241" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2242">
+      <c r="A2242" t="n">
+        <v>1460602</v>
+      </c>
+      <c r="B2242" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2242" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2242" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2242" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2242" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2242" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2243">
+      <c r="A2243" t="n">
+        <v>1460603</v>
+      </c>
+      <c r="B2243" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2243" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2243" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2243" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2243" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2243" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2244">
+      <c r="A2244" t="n">
+        <v>1460684</v>
+      </c>
+      <c r="B2244" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2244" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2244" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2244" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2244" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2244" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2245">
+      <c r="A2245" t="n">
+        <v>1460685</v>
+      </c>
+      <c r="B2245" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2245" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2245" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2245" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2245" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2245" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2246">
+      <c r="A2246" t="n">
+        <v>1460686</v>
+      </c>
+      <c r="B2246" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2246" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2246" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2246" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2246" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2246" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2247">
+      <c r="A2247" t="n">
+        <v>1460694</v>
+      </c>
+      <c r="B2247" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2247" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2247" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2247" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2247" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2247" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2248">
+      <c r="A2248" t="n">
+        <v>1460695</v>
+      </c>
+      <c r="B2248" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2248" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2248" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2248" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2248" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2248" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2249">
+      <c r="A2249" t="n">
+        <v>1460696</v>
+      </c>
+      <c r="B2249" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2249" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2249" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2249" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2249" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2249" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2250">
+      <c r="A2250" t="n">
+        <v>1460697</v>
+      </c>
+      <c r="B2250" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2250" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2250" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2250" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2250" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2250" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2251">
+      <c r="A2251" t="n">
+        <v>1460755</v>
+      </c>
+      <c r="B2251" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2251" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2251" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2251" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2251" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2251" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2252">
+      <c r="A2252" t="n">
+        <v>1460756</v>
+      </c>
+      <c r="B2252" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2252" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2252" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2252" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2252" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2252" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2253">
+      <c r="A2253" t="n">
+        <v>1460757</v>
+      </c>
+      <c r="B2253" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2253" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2253" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2253" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2253" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2253" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2254">
+      <c r="A2254" t="n">
+        <v>1460758</v>
+      </c>
+      <c r="B2254" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2254" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2254" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2254" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2254" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2254" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2255">
+      <c r="A2255" t="n">
+        <v>1460809</v>
+      </c>
+      <c r="B2255" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2255" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2255" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2255" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2255" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2255" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2256">
+      <c r="A2256" t="n">
+        <v>1460810</v>
+      </c>
+      <c r="B2256" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2256" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2256" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2256" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2256" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2256" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2257">
+      <c r="A2257" t="n">
+        <v>1460811</v>
+      </c>
+      <c r="B2257" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2257" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2257" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2257" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2257" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2257" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2258">
+      <c r="A2258" t="n">
+        <v>1460812</v>
+      </c>
+      <c r="B2258" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2258" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2258" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2258" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2258" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2258" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2259">
+      <c r="A2259" t="n">
+        <v>1460830</v>
+      </c>
+      <c r="B2259" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2259" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2259" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2259" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2259" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2259" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2260">
+      <c r="A2260" t="n">
+        <v>1460831</v>
+      </c>
+      <c r="B2260" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2260" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2260" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2260" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2260" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2260" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2261">
+      <c r="A2261" t="n">
+        <v>1460832</v>
+      </c>
+      <c r="B2261" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2261" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2261" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2261" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2261" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2261" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2262">
+      <c r="A2262" t="n">
+        <v>1460863</v>
+      </c>
+      <c r="B2262" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2262" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2262" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2262" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2262" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2262" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2263">
+      <c r="A2263" t="n">
+        <v>1460864</v>
+      </c>
+      <c r="B2263" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2263" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2263" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2263" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2263" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2263" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2264">
+      <c r="A2264" t="n">
+        <v>1460865</v>
+      </c>
+      <c r="B2264" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2264" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2264" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2264" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2264" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2264" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2265">
+      <c r="A2265" t="n">
+        <v>1460882</v>
+      </c>
+      <c r="B2265" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2265" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2265" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2265" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2265" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2265" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2266">
+      <c r="A2266" t="n">
+        <v>1460883</v>
+      </c>
+      <c r="B2266" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2266" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2266" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2266" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2266" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2266" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2267">
+      <c r="A2267" t="n">
+        <v>1460884</v>
+      </c>
+      <c r="B2267" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2267" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2267" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2267" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2267" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2267" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2268">
+      <c r="A2268" t="n">
+        <v>1460885</v>
+      </c>
+      <c r="B2268" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2268" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2268" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2268" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2268" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2268" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2269">
+      <c r="A2269" t="n">
+        <v>1461057</v>
+      </c>
+      <c r="B2269" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2269" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2269" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2269" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2269" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2269" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2270">
+      <c r="A2270" t="n">
+        <v>1461058</v>
+      </c>
+      <c r="B2270" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2270" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2270" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2270" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2270" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2270" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2271">
+      <c r="A2271" t="n">
+        <v>1461059</v>
+      </c>
+      <c r="B2271" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2271" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2271" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2271" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2271" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2271" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2272">
+      <c r="A2272" t="n">
+        <v>1468958</v>
+      </c>
+      <c r="B2272" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2272" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2272" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2272" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2272" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2272" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2273">
+      <c r="A2273" t="n">
+        <v>1468959</v>
+      </c>
+      <c r="B2273" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2273" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2273" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2273" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2273" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2273" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2274">
+      <c r="A2274" t="n">
+        <v>1469006</v>
+      </c>
+      <c r="B2274" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2274" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2274" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2274" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2274" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2274" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2275">
+      <c r="A2275" t="n">
+        <v>1469007</v>
+      </c>
+      <c r="B2275" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2275" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2275" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2275" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2275" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2275" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2276">
+      <c r="A2276" t="n">
+        <v>1469008</v>
+      </c>
+      <c r="B2276" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2276" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2276" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2276" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2276" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2276" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" t="n">
+        <v>1469043</v>
+      </c>
+      <c r="B2277" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2277" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2277" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2277" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2277" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2277" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" t="n">
+        <v>1469044</v>
+      </c>
+      <c r="B2278" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2278" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2278" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2278" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2278" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2278" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" t="n">
+        <v>1469045</v>
+      </c>
+      <c r="B2279" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2279" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2279" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2279" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2279" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2279" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" t="n">
+        <v>1469058</v>
+      </c>
+      <c r="B2280" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2280" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2280" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2280" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2280" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2280" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" t="n">
+        <v>1469059</v>
+      </c>
+      <c r="B2281" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2281" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2281" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2281" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2281" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2281" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" t="n">
+        <v>1469082</v>
+      </c>
+      <c r="B2282" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2282" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2282" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2282" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2282" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2282" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" t="n">
+        <v>1469083</v>
+      </c>
+      <c r="B2283" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2283" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2283" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2283" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2283" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2283" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" t="n">
+        <v>1469099</v>
+      </c>
+      <c r="B2284" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2284" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2284" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2284" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2284" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2284" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" t="n">
+        <v>1469100</v>
+      </c>
+      <c r="B2285" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2285" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2285" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2285" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2285" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2285" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" t="n">
+        <v>1469101</v>
+      </c>
+      <c r="B2286" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2286" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2286" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2286" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2286" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2286" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" t="n">
+        <v>1469236</v>
+      </c>
+      <c r="B2287" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2287" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2287" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2287" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2287" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2287" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" t="n">
+        <v>1469237</v>
+      </c>
+      <c r="B2288" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2288" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2288" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2288" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2288" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2288" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" t="n">
+        <v>1469238</v>
+      </c>
+      <c r="B2289" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2289" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2289" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2289" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2289" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2289" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" t="n">
+        <v>1469239</v>
+      </c>
+      <c r="B2290" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2290" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2290" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2290" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2290" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2290" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" t="n">
+        <v>1469319</v>
+      </c>
+      <c r="B2291" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2291" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2291" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2291" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2291" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2291" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" t="n">
+        <v>1469320</v>
+      </c>
+      <c r="B2292" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2292" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2292" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2292" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2292" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2292" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" t="n">
+        <v>1469321</v>
+      </c>
+      <c r="B2293" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2293" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2293" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2293" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2293" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2293" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" t="n">
+        <v>1469423</v>
+      </c>
+      <c r="B2294" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2294" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2294" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2294" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2294" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2294" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" t="n">
+        <v>1469424</v>
+      </c>
+      <c r="B2295" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2295" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2295" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2295" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2295" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2295" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" t="n">
+        <v>1469425</v>
+      </c>
+      <c r="B2296" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2296" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2296" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2296" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2296" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2296" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="n">
+        <v>1469474</v>
+      </c>
+      <c r="B2297" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2297" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2297" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2297" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2297" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2297" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" t="n">
+        <v>1469475</v>
+      </c>
+      <c r="B2298" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2298" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2298" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2298" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2298" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2298" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" t="n">
+        <v>1469476</v>
+      </c>
+      <c r="B2299" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2299" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2299" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2299" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2299" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2299" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" t="n">
+        <v>1469575</v>
+      </c>
+      <c r="B2300" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2300" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2300" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2300" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2300" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2300" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" t="n">
+        <v>1469576</v>
+      </c>
+      <c r="B2301" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2301" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2301" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2301" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2301" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2301" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" t="n">
+        <v>1469577</v>
+      </c>
+      <c r="B2302" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2302" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2302" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2302" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2302" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2302" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" t="n">
+        <v>1469582</v>
+      </c>
+      <c r="B2303" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2303" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2303" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2303" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2303" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2303" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" t="n">
+        <v>1460456</v>
+      </c>
+      <c r="B2304" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2304" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2304" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2304" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2304" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2304" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" t="n">
+        <v>1460457</v>
+      </c>
+      <c r="B2305" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2305" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2305" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2305" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2305" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2305" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" t="n">
+        <v>1460458</v>
+      </c>
+      <c r="B2306" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2306" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2306" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2306" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2306" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2306" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" t="n">
+        <v>1460459</v>
+      </c>
+      <c r="B2307" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2307" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2307" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2307" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2307" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2307" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" t="n">
+        <v>1460463</v>
+      </c>
+      <c r="B2308" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2308" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2308" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2308" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2308" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2308" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" t="n">
+        <v>1460464</v>
+      </c>
+      <c r="B2309" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2309" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2309" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2309" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2309" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2309" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" t="n">
+        <v>1460465</v>
+      </c>
+      <c r="B2310" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2310" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2310" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2310" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2310" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2310" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" t="n">
+        <v>1460607</v>
+      </c>
+      <c r="B2311" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2311" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2311" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2311" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2311" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2311" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" t="n">
+        <v>1460608</v>
+      </c>
+      <c r="B2312" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2312" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2312" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2312" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2312" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2312" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" t="n">
+        <v>1460609</v>
+      </c>
+      <c r="B2313" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2313" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2313" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2313" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2313" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2313" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" t="n">
+        <v>1460690</v>
+      </c>
+      <c r="B2314" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2314" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2314" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2314" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2314" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2314" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" t="n">
+        <v>1460691</v>
+      </c>
+      <c r="B2315" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2315" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2315" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2315" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2315" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2315" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" t="n">
+        <v>1460692</v>
+      </c>
+      <c r="B2316" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2316" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2316" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2316" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2316" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2316" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" t="n">
+        <v>1460693</v>
+      </c>
+      <c r="B2317" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
+      <c r="C2317" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2317" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2317" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2317" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2317" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
rodado nos dois computadores
</commit_message>
<xml_diff>
--- a/BASE_DADOS.xlsx
+++ b/BASE_DADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2319"/>
+  <dimension ref="A1:G2320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -74492,6 +74492,41 @@
         </is>
       </c>
     </row>
+    <row r="2320">
+      <c r="A2320" t="n">
+        <v>1469201</v>
+      </c>
+      <c r="B2320" t="inlineStr">
+        <is>
+          <t>27/05/2024</t>
+        </is>
+      </c>
+      <c r="C2320" t="inlineStr">
+        <is>
+          <t>04/06/202422:00</t>
+        </is>
+      </c>
+      <c r="D2320" t="inlineStr">
+        <is>
+          <t>04/06/202422:01</t>
+        </is>
+      </c>
+      <c r="E2320" t="inlineStr">
+        <is>
+          <t>04/06/202422:02</t>
+        </is>
+      </c>
+      <c r="F2320" t="inlineStr">
+        <is>
+          <t>Entregue</t>
+        </is>
+      </c>
+      <c r="G2320" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>